<commit_message>
fixed all data parsing, the data is now parsed from the excel sheet according to cough cough data[sheet(no)][row(no)][col(no)], its finaly done
</commit_message>
<xml_diff>
--- a/Backend/uploads/app_sug_2.xlsx
+++ b/Backend/uploads/app_sug_2.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="626" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14940" tabRatio="964"/>
   </bookViews>
   <sheets>
-    <sheet name="MDI advice before planned ex" sheetId="1" r:id="rId1"/>
-    <sheet name="MDI advice after planned ex" sheetId="2" r:id="rId2"/>
-    <sheet name="MDI advice before unplanned ex" sheetId="3" r:id="rId3"/>
-    <sheet name="MDI advice after unplanned ex" sheetId="4" r:id="rId4"/>
-    <sheet name="Pump advice before planned ex" sheetId="5" r:id="rId5"/>
-    <sheet name="Pump advice after planned ex" sheetId="6" r:id="rId6"/>
-    <sheet name="PUMP advice before unplanned ex" sheetId="7" r:id="rId7"/>
-    <sheet name="Pump advice after unplanned ex" sheetId="8" r:id="rId8"/>
-    <sheet name="Links to advice " sheetId="9" r:id="rId9"/>
+    <sheet name="MDIadviceBeforePlannedEx" sheetId="1" r:id="rId1"/>
+    <sheet name="MDIadviceAfterPlannedEx" sheetId="2" r:id="rId2"/>
+    <sheet name="MDIadviceBeforeUnplannedEx" sheetId="3" r:id="rId3"/>
+    <sheet name="MDIadviceAfterUnplannedEx" sheetId="4" r:id="rId4"/>
+    <sheet name="PumpAdviceBeforePlannedEx" sheetId="5" r:id="rId5"/>
+    <sheet name="PumpAdviceAfterPlannedEx" sheetId="6" r:id="rId6"/>
+    <sheet name="PumpAdviceBeforeUnplannedEx" sheetId="7" r:id="rId7"/>
+    <sheet name="PumpAdviceAfterUnplannedEx" sheetId="8" r:id="rId8"/>
+    <sheet name="LinksToAdvice" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="206">
   <si>
     <r>
       <rPr>
@@ -1648,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
-    <sheetView topLeftCell="H54" workbookViewId="0">
-      <selection activeCell="S68" sqref="S1:W68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1658,7 +1658,7 @@
     <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="5" max="5" width="57.33203125" customWidth="1"/>
     <col min="6" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1965,7 +1965,9 @@
       <c r="C33" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E33" s="2" t="s">
         <v>5</v>
       </c>
@@ -4858,7 +4860,9 @@
       <c r="C56" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D56" s="22"/>
+      <c r="D56" s="22" t="s">
+        <v>4</v>
+      </c>
       <c r="E56" s="22" t="s">
         <v>5</v>
       </c>
@@ -5315,7 +5319,7 @@
   <dimension ref="A1:X68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6025,7 +6029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
@@ -7158,7 +7162,8 @@
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" customWidth="1"/>
+    <col min="5" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15">
@@ -8208,7 +8213,7 @@
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>